<commit_message>
Ajout de nouvelles sources
</commit_message>
<xml_diff>
--- a/data/donnees_insee.xlsx
+++ b/data/donnees_insee.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="118">
   <si>
     <t xml:space="preserve">Emploi salarié total</t>
   </si>
@@ -498,6 +498,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.insee.fr/fr/statistiques/serie/010759955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.insee.fr/fr/statistiques/serie/010760300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.insee.fr/fr/statistiques/serie/010759801</t>
   </si>
 </sst>
 </file>
@@ -702,7 +708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -807,6 +813,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +889,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -909,8 +919,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.300432365657813"/>
-          <c:y val="0.035364768683274"/>
+          <c:x val="0.300481362626512"/>
+          <c:y val="0.0353687020353687"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1251,11 +1261,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="91969723"/>
-        <c:axId val="25597113"/>
+        <c:axId val="91986482"/>
+        <c:axId val="53941213"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91969723"/>
+        <c:axId val="91986482"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,7 +1293,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25597113"/>
+        <c:crossAx val="53941213"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1291,7 +1301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25597113"/>
+        <c:axId val="53941213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1338,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91969723"/>
+        <c:crossAx val="91986482"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1387,9 +1397,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>100</xdr:col>
-      <xdr:colOff>127080</xdr:colOff>
+      <xdr:colOff>126720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1397,8 +1407,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="78633360" y="2813400"/>
-        <a:ext cx="5828040" cy="3236760"/>
+        <a:off x="78685200" y="2813400"/>
+        <a:ext cx="5833080" cy="3236400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1419,10 +1429,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A14:B14 B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
@@ -2056,10 +2066,10 @@
   <dimension ref="A1:CH42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="A14:B14 A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.33"/>
@@ -3147,10 +3157,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A14:B14 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="918" style="0" width="11.52"/>
@@ -3725,10 +3735,10 @@
   <dimension ref="A7:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="A14:B14 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.58"/>
   </cols>
@@ -4269,15 +4279,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="179.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.06"/>
   </cols>
   <sheetData>
@@ -4370,7 +4380,23 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="25"/>
+      <c r="A12" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="25" t="n">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4391,10 +4417,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="1" sqref="A14:B14 I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.55"/>
   </cols>
@@ -5022,10 +5048,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="A14:B14 C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.4"/>
   </cols>
@@ -5656,10 +5682,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BX1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CH8" activeCellId="0" sqref="CH8"/>
+      <selection pane="topLeft" activeCell="CH8" activeCellId="1" sqref="A14:B14 CH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.33"/>
@@ -6300,10 +6326,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BV9" activeCellId="0" sqref="BV9"/>
+      <selection pane="topLeft" activeCell="BV9" activeCellId="1" sqref="A14:B14 BV9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="918" style="0" width="11.52"/>
@@ -6878,10 +6904,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="A14:B14 C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.88"/>
   </cols>
@@ -7512,10 +7538,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A14:B14 A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
   </cols>
@@ -8147,10 +8173,10 @@
   <dimension ref="A1:CH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A14:B14 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
   </cols>
@@ -8782,10 +8808,10 @@
   <dimension ref="A1:CH41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A14:B14 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.33"/>

</xml_diff>